<commit_message>
Fix Melbourne sparse data
</commit_message>
<xml_diff>
--- a/evaluation/sparse_data.xlsx
+++ b/evaluation/sparse_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Vortraege\2022\FluidFlowerBenchmarkWorkshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C862B3F-B9B5-458C-8C04-6A33AABBAC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A3820B-EFCB-401B-8B80-2296C4939379}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="1" activeTab="9" xr2:uid="{6E0CDC08-98CA-4B3E-9EF0-0B30DDB70824}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="1" activeTab="7" xr2:uid="{6E0CDC08-98CA-4B3E-9EF0-0B30DDB70824}"/>
   </bookViews>
   <sheets>
     <sheet name="Austin" sheetId="1" r:id="rId1"/>
@@ -964,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61105E5E-A45E-4949-AEF5-EE713A12D2E3}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -3645,8 +3645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3B9647-CC6A-45EF-9900-9890175E4B9A}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3691,36 +3691,48 @@
         <v>6</v>
       </c>
       <c r="B2" s="6">
-        <v>112105.8</v>
+        <v>111709.5425</v>
       </c>
       <c r="C2" s="7">
-        <v>112217</v>
+        <v>112375.7389</v>
       </c>
       <c r="D2" s="6">
-        <v>112284.3</v>
+        <v>112880.9439</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
+      <c r="F2" s="6">
+        <v>354.74570590000002</v>
+      </c>
+      <c r="G2" s="7">
+        <v>275.12807959999998</v>
+      </c>
+      <c r="H2" s="6">
+        <v>306.4205336</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6">
-        <v>105255</v>
+        <v>104734.02650000001</v>
       </c>
       <c r="C3" s="7">
-        <v>105255</v>
+        <v>105222.6039</v>
       </c>
       <c r="D3" s="6">
-        <v>105317.1</v>
+        <v>105793.79580000001</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
+      <c r="F3" s="6">
+        <v>236.0989309</v>
+      </c>
+      <c r="G3" s="7">
+        <v>187.6438417</v>
+      </c>
+      <c r="H3" s="6">
+        <v>278.69779690000001</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -3737,18 +3749,24 @@
         <v>8</v>
       </c>
       <c r="B5" s="6">
-        <v>18000</v>
+        <v>15984.173059999999</v>
       </c>
       <c r="C5" s="7">
-        <v>18000</v>
+        <v>17092.620699999999</v>
       </c>
       <c r="D5" s="6">
-        <v>18000</v>
+        <v>17897.945329999999</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="6">
+        <v>74.064079370000002</v>
+      </c>
+      <c r="G5" s="7">
+        <v>322.99627889999999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>119.69559340000001</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
@@ -3765,18 +3783,24 @@
         <v>9</v>
       </c>
       <c r="B7" s="6">
-        <v>5.4856200000000005E-4</v>
+        <v>4.0232799999999997E-4</v>
       </c>
       <c r="C7" s="7">
-        <v>1.5672100000000001E-3</v>
+        <v>5.8297100000000005E-4</v>
       </c>
       <c r="D7" s="6">
-        <v>1.5795900000000001E-3</v>
+        <v>7.50302E-4</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
+      <c r="F7" s="6">
+        <v>1.8300000000000001E-5</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3.8399999999999998E-5</v>
+      </c>
+      <c r="H7" s="6">
+        <v>6.0399999999999998E-5</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
@@ -3792,22 +3816,28 @@
         <v>0</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6">
-        <v>3.8247390000000002E-3</v>
+        <v>3.6448349999999999E-3</v>
       </c>
       <c r="C9" s="7">
-        <v>5.3423699999999999E-3</v>
+        <v>3.8843380000000002E-3</v>
       </c>
       <c r="D9" s="6">
-        <v>5.998148E-3</v>
+        <v>4.2781520000000003E-3</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3819,18 +3849,24 @@
         <v>15</v>
       </c>
       <c r="B10" s="6">
-        <v>6.6722099999999996E-4</v>
+        <v>6.66583E-4</v>
       </c>
       <c r="C10" s="7">
         <v>7.5796200000000005E-4</v>
       </c>
       <c r="D10" s="6">
+        <v>8.57116E-4</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>6.6722099999999996E-4</v>
+      </c>
+      <c r="G10" s="7">
+        <v>7.5796200000000005E-4</v>
+      </c>
+      <c r="H10" s="6">
         <v>8.5354300000000001E-4</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
@@ -3847,13 +3883,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>1.4851000000000001E-18</v>
+        <v>3.1599999999999998E-17</v>
       </c>
       <c r="C12" s="7">
-        <v>2.96104E-18</v>
+        <v>3.39E-17</v>
       </c>
       <c r="D12" s="6">
-        <v>3.4005399999999999E-17</v>
+        <v>3.8099999999999999E-17</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -3883,13 +3919,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <v>1.8609699999999999E-5</v>
+        <v>1.5702730000000001E-3</v>
       </c>
       <c r="C14" s="7">
-        <v>2.7756700000000001E-5</v>
+        <v>1.611407E-3</v>
       </c>
       <c r="D14" s="6">
-        <v>1.613047E-3</v>
+        <v>1.619606E-3</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -3901,13 +3937,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="6">
-        <v>2.57976E-6</v>
+        <v>2.5799999999999999E-6</v>
       </c>
       <c r="C15" s="7">
-        <v>3.8091600000000001E-6</v>
+        <v>3.8099999999999999E-6</v>
       </c>
       <c r="D15" s="6">
-        <v>2.34433E-5</v>
+        <v>2.34E-5</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3938,9 +3974,15 @@
         <v>14023.2197</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
+      <c r="F17" s="6">
+        <v>125.9389721</v>
+      </c>
+      <c r="G17" s="7">
+        <v>152.95976490000001</v>
+      </c>
+      <c r="H17" s="6">
+        <v>268.41984600000001</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
@@ -3978,6 +4020,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>